<commit_message>
refactor: update import templates with additional fields and add validation for import of new fields using column mapping and data validation feature
</commit_message>
<xml_diff>
--- a/public/xlsx/chemical_import_template.xlsx
+++ b/public/xlsx/chemical_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F548E0-5EE9-4BEA-9836-AD91F2BDA593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7933276A-4E92-4F51-A09C-A4A7BEB354DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_chemicals" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>decoupled</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>expiration date</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>solubility</t>
+  </si>
+  <si>
+    <t>inventory label</t>
   </si>
 </sst>
 </file>
@@ -595,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:AA1048576"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,51 +626,52 @@
     <col min="10" max="10" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="255" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.140625" customWidth="1"/>
-    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="22.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="255" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.140625" customWidth="1"/>
+    <col min="38" max="38" width="18" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="18" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="18.28515625" customWidth="1"/>
+    <col min="55" max="55" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -696,139 +709,151 @@
         <v>52</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
+    <row r="2" spans="1:59" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: export-import of additional sample properties (#2906)
* feat: allow import of form - solubility - color - inventory_label using sdf and xlsx formats

* refactor: update import templates with additional fields and add validation for import of new fields using column mapping and data validation feature
</commit_message>
<xml_diff>
--- a/public/xlsx/chemical_import_template.xlsx
+++ b/public/xlsx/chemical_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F548E0-5EE9-4BEA-9836-AD91F2BDA593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7933276A-4E92-4F51-A09C-A4A7BEB354DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_chemicals" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>decoupled</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>expiration date</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>solubility</t>
+  </si>
+  <si>
+    <t>inventory label</t>
   </si>
 </sst>
 </file>
@@ -595,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:AA1048576"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,51 +626,52 @@
     <col min="10" max="10" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="255" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.140625" customWidth="1"/>
-    <col min="34" max="34" width="18" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="22.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="255" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.140625" customWidth="1"/>
+    <col min="38" max="38" width="18" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="18" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="18.28515625" customWidth="1"/>
+    <col min="55" max="55" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -696,139 +709,151 @@
         <v>52</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BG1" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
+    <row r="2" spans="1:59" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>